<commit_message>
working in the matching names of crops
</commit_message>
<xml_diff>
--- a/data/conf/crops.xlsx
+++ b/data/conf/crops.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\itpgrfa_crop_indicator_code\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C8EA75BF-BC23-4CA4-8E45-909AF081B0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B2935B-3FDD-4890-AEDC-55CF5F5FF853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="crops" sheetId="1" r:id="rId1"/>
-    <sheet name="crops_fao" sheetId="2" r:id="rId2"/>
+    <sheet name="fao" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="807">
   <si>
     <t>name</t>
   </si>
@@ -2442,15 +2442,12 @@
   </si>
   <si>
     <t>fao</t>
-  </si>
-  <si>
-    <t>crop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3284,7 +3281,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B356"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6150,11 +6147,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C495"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6165,7 +6162,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>807</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>806</v>

</xml_diff>